<commit_message>
implmented hook : pytest_generate_tests
</commit_message>
<xml_diff>
--- a/TestData/logintestdata.xlsx
+++ b/TestData/logintestdata.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CB5141-7411-4D44-BDA6-E0335A906176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -53,13 +55,16 @@
   </si>
   <si>
     <t>dmin@yourstore.com</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +79,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,9 +108,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -119,9 +133,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,9 +173,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,7 +210,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,7 +245,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -404,20 +418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -439,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -450,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -461,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -474,11 +488,63 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB3B997-67B7-44CA-AC3D-347CFF4E58D8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>